<commit_message>
fix: Refactor rendering logic in RenderActivityPlanSheet and update template file
</commit_message>
<xml_diff>
--- a/public/assets/file/Template Activity Plan.xlsx
+++ b/public/assets/file/Template Activity Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\core\public\assets\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCF115E-3914-47D6-90DF-FCEE21036DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB0CCBC-F01D-44A4-9F93-E1621C88BC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -120,7 +120,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmmm\ d\,\ yyyy"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,13 +151,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -580,9 +573,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -633,9 +626,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -658,22 +648,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -681,11 +683,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -698,20 +700,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -976,8 +966,8 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="51" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="51" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -998,12 +988,12 @@
   <sheetData>
     <row r="1" spans="1:24" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="12"/>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="31"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1026,10 +1016,10 @@
     </row>
     <row r="2" spans="1:24" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10"/>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="52"/>
+      <c r="C2" s="27"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -1200,39 +1190,39 @@
     </row>
     <row r="8" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10"/>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="39" t="s">
+      <c r="D8" s="43"/>
+      <c r="E8" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="39" t="s">
+      <c r="F8" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="39" t="s">
+      <c r="G8" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="H8" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="32" t="s">
+      <c r="I8" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
-      <c r="Q8" s="28"/>
-      <c r="R8" s="28"/>
-      <c r="S8" s="28"/>
-      <c r="T8" s="33"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="31"/>
+      <c r="T8" s="36"/>
       <c r="U8" s="15"/>
       <c r="V8" s="11"/>
       <c r="W8" s="11"/>
@@ -1240,25 +1230,25 @@
     </row>
     <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="35"/>
-      <c r="O9" s="35"/>
-      <c r="P9" s="35"/>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="35"/>
-      <c r="S9" s="35"/>
-      <c r="T9" s="36"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="38"/>
+      <c r="R9" s="38"/>
+      <c r="S9" s="38"/>
+      <c r="T9" s="39"/>
       <c r="U9" s="15"/>
       <c r="V9" s="11"/>
       <c r="W9" s="11"/>
@@ -1266,13 +1256,13 @@
     </row>
     <row r="10" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="10"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
       <c r="I10" s="8" t="s">
         <v>12</v>
       </c>
@@ -1316,25 +1306,25 @@
     </row>
     <row r="11" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10"/>
-      <c r="B11" s="45"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="46"/>
-      <c r="M11" s="46"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="46"/>
-      <c r="Q11" s="46"/>
-      <c r="R11" s="46"/>
-      <c r="S11" s="46"/>
-      <c r="T11" s="47"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="49"/>
+      <c r="P11" s="49"/>
+      <c r="Q11" s="49"/>
+      <c r="R11" s="49"/>
+      <c r="S11" s="49"/>
+      <c r="T11" s="50"/>
       <c r="U11" s="15"/>
       <c r="V11" s="11"/>
       <c r="W11" s="11"/>
@@ -1342,25 +1332,25 @@
     </row>
     <row r="12" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25"/>
-      <c r="T12" s="26"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="24"/>
+      <c r="S12" s="24"/>
+      <c r="T12" s="25"/>
       <c r="U12" s="15"/>
       <c r="V12" s="11"/>
       <c r="W12" s="11"/>
@@ -1401,18 +1391,18 @@
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="20"/>
-      <c r="S14" s="20"/>
-      <c r="T14" s="20"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
       <c r="U14" s="15"/>
       <c r="V14" s="11"/>
       <c r="W14" s="11"/>
@@ -1531,18 +1521,18 @@
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
       <c r="L19" s="11"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
       <c r="Q19" s="11"/>
-      <c r="R19" s="20"/>
-      <c r="S19" s="20"/>
-      <c r="T19" s="20"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="19"/>
+      <c r="T19" s="19"/>
       <c r="U19" s="15"/>
       <c r="V19" s="11"/>
       <c r="W19" s="11"/>
@@ -1579,7 +1569,7 @@
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
-      <c r="E21" s="18"/>
+      <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="16"/>
@@ -1683,7 +1673,7 @@
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
-      <c r="E25" s="19"/>
+      <c r="E25" s="18"/>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
@@ -1709,7 +1699,7 @@
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
-      <c r="E26" s="19"/>
+      <c r="E26" s="18"/>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
@@ -1735,7 +1725,7 @@
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
-      <c r="E27" s="19"/>
+      <c r="E27" s="18"/>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
@@ -1761,7 +1751,7 @@
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
-      <c r="E28" s="19"/>
+      <c r="E28" s="18"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
@@ -1787,7 +1777,7 @@
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
-      <c r="E29" s="19"/>
+      <c r="E29" s="18"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
@@ -1813,7 +1803,7 @@
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
-      <c r="E30" s="19"/>
+      <c r="E30" s="18"/>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
@@ -1839,7 +1829,7 @@
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
-      <c r="E31" s="19"/>
+      <c r="E31" s="18"/>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
       <c r="H31" s="11"/>

</xml_diff>